<commit_message>
1 GUI 2 IGUI added GUI and added logic to add items and scoops
</commit_message>
<xml_diff>
--- a/P06/Scrum_MICE_Sprint_2.xlsx
+++ b/P06/Scrum_MICE_Sprint_2.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30813DE8-43D6-4FF3-9767-23B504E9B7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P06/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21905E1B-200D-F946-8BCD-5D7D8A2F9E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22840" yWindow="500" windowWidth="28360" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="195">
   <si>
     <t>Product Name:</t>
   </si>
@@ -580,6 +585,48 @@
   </si>
   <si>
     <t>IMPORTANT: This is an optional sprint for students seeking additional points</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 1</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 2</t>
+  </si>
+  <si>
+    <t>Team Move Detroit To Ohio</t>
+  </si>
+  <si>
+    <t>Rishabh Mediratta</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Create IceCreamFlavor class extending Item and add constructor</t>
+  </si>
+  <si>
+    <t>Completed Day 6</t>
+  </si>
+  <si>
+    <t>Create MixInFlavor class extending Item and add constructor</t>
+  </si>
+  <si>
+    <t>Create MixIn and add constructor and toString method</t>
+  </si>
+  <si>
+    <t>Create Scoop class and add constructor, addMixIn and override toString methods</t>
+  </si>
+  <si>
+    <t>Add TestScoop to test Scoop</t>
+  </si>
+  <si>
+    <t>Fix conditions to check if mixins ArrayList is not initialized</t>
+  </si>
+  <si>
+    <t>Made a GUI instead of using a terminal</t>
+  </si>
+  <si>
+    <t>Added logic to GUI to make items and scoops</t>
   </si>
 </sst>
 </file>
@@ -1031,22 +1078,22 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,7 +1300,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1330,28 +1377,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,7 +1448,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1475,7 +1522,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -1566,7 +1613,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1643,28 +1690,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,7 +1761,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1788,7 +1835,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3129,7 +3176,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -3170,7 +3217,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
@@ -3211,7 +3258,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
@@ -3252,7 +3299,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
@@ -3293,7 +3340,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
@@ -3334,7 +3381,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
@@ -3375,7 +3422,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
@@ -3701,27 +3748,27 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B63"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="45.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="39.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="53.7109375" style="3" customWidth="1"/>
-    <col min="12" max="1024" width="11.5703125" style="3"/>
+    <col min="3" max="3" width="8.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="45.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="53.6640625" style="3" customWidth="1"/>
+    <col min="12" max="1024" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="17.45">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3739,11 +3786,13 @@
       </c>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="15">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="16">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="30" t="s">
+        <v>183</v>
+      </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
@@ -3787,14 +3836,20 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="31" t="s">
+        <v>184</v>
+      </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1002035684</v>
+      </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1">
@@ -3903,12 +3958,12 @@
         <v>1</v>
       </c>
       <c r="B13" s="4">
-        <f>B12-C13</f>
-        <v>40</v>
+        <f t="shared" ref="B13:B18" si="0">B12-C13</f>
+        <v>36</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 1")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="4"/>
@@ -3927,12 +3982,12 @@
         <v>2</v>
       </c>
       <c r="B14" s="4">
-        <f>B13-C14</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="4"/>
@@ -3951,8 +4006,8 @@
         <v>3</v>
       </c>
       <c r="B15" s="4">
-        <f>B14-C15</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
@@ -3975,8 +4030,8 @@
         <v>4</v>
       </c>
       <c r="B16" s="4">
-        <f>B15-C16</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -3995,8 +4050,8 @@
         <v>5</v>
       </c>
       <c r="B17" s="4">
-        <f>B16-C17</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -4015,8 +4070,8 @@
         <v>6</v>
       </c>
       <c r="B18" s="4">
-        <f>B17-C18</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -4119,7 +4174,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="14">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -4133,8 +4188,12 @@
       <c r="E24" s="9">
         <v>5</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="F24" s="14">
+        <v>1</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="H24" s="12" t="s">
         <v>31</v>
       </c>
@@ -4148,7 +4207,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="14">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -4162,8 +4221,12 @@
       <c r="E25" s="9">
         <v>1</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="H25" s="12" t="s">
         <v>31</v>
       </c>
@@ -4177,7 +4240,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="23.85">
+    <row r="26" spans="1:11" ht="28">
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
@@ -4191,8 +4254,12 @@
       <c r="E26" s="9">
         <v>2</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="F26" s="14">
+        <v>1</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="H26" s="12" t="s">
         <v>31</v>
       </c>
@@ -4206,7 +4273,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="23.85">
+    <row r="27" spans="1:11" ht="28">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -4220,8 +4287,12 @@
       <c r="E27" s="9">
         <v>13</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="F27" s="14">
+        <v>1</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="H27" s="12" t="s">
         <v>31</v>
       </c>
@@ -4235,7 +4306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="24">
+    <row r="28" spans="1:11" ht="28">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -4249,8 +4320,12 @@
       <c r="E28" s="9">
         <v>13</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="F28" s="14">
+        <v>2</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>182</v>
+      </c>
       <c r="H28" s="12" t="s">
         <v>31</v>
       </c>
@@ -4264,7 +4339,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="14">
       <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
@@ -4278,8 +4353,12 @@
       <c r="E29" s="9">
         <v>13</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="F29" s="14">
+        <v>2</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>182</v>
+      </c>
       <c r="H29" s="12" t="s">
         <v>31</v>
       </c>
@@ -4293,7 +4372,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="23.85">
+    <row r="30" spans="1:11" ht="28">
       <c r="A30" s="3" t="s">
         <v>53</v>
       </c>
@@ -4322,7 +4401,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" ht="14">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
@@ -4351,7 +4430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="16" customFormat="1">
+    <row r="32" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A32" s="3" t="s">
         <v>61</v>
       </c>
@@ -4378,7 +4457,7 @@
       </c>
       <c r="K32" s="15"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" ht="14">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -4405,7 +4484,7 @@
       </c>
       <c r="K33" s="15"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" ht="14">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -4432,7 +4511,7 @@
       </c>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" ht="23.85">
+    <row r="35" spans="1:11" ht="28">
       <c r="A35" s="3" t="s">
         <v>70</v>
       </c>
@@ -4461,7 +4540,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="23.85">
+    <row r="36" spans="1:11" ht="28">
       <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
@@ -4490,7 +4569,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="16" customFormat="1">
+    <row r="37" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A37" s="3" t="s">
         <v>78</v>
       </c>
@@ -4517,7 +4596,7 @@
       </c>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="16" customFormat="1">
+    <row r="38" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A38" s="3" t="s">
         <v>81</v>
       </c>
@@ -4544,7 +4623,7 @@
       </c>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="16" customFormat="1">
+    <row r="39" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A39" s="3" t="s">
         <v>84</v>
       </c>
@@ -4571,7 +4650,7 @@
       </c>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="16" customFormat="1" ht="23.85">
+    <row r="40" spans="1:11" s="16" customFormat="1" ht="28">
       <c r="A40" s="3" t="s">
         <v>87</v>
       </c>
@@ -4600,7 +4679,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="16" customFormat="1">
+    <row r="41" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A41" s="3" t="s">
         <v>91</v>
       </c>
@@ -4629,7 +4708,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="16" customFormat="1" ht="23.85">
+    <row r="42" spans="1:11" s="16" customFormat="1" ht="28">
       <c r="A42" s="3" t="s">
         <v>93</v>
       </c>
@@ -4685,7 +4764,7 @@
       </c>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="16" customFormat="1" ht="23.85">
+    <row r="44" spans="1:11" s="16" customFormat="1" ht="28">
       <c r="A44" s="3" t="s">
         <v>100</v>
       </c>
@@ -4714,7 +4793,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="16" customFormat="1" ht="23.85">
+    <row r="45" spans="1:11" s="16" customFormat="1" ht="28">
       <c r="A45" s="3" t="s">
         <v>104</v>
       </c>
@@ -4743,7 +4822,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="23.85">
+    <row r="46" spans="1:11" ht="28">
       <c r="A46" s="3" t="s">
         <v>108</v>
       </c>
@@ -4772,7 +4851,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" ht="14">
       <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
@@ -4797,7 +4876,7 @@
       </c>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="16" customFormat="1">
+    <row r="48" spans="1:11" s="16" customFormat="1" ht="14">
       <c r="A48" s="3" t="s">
         <v>114</v>
       </c>
@@ -4822,7 +4901,7 @@
       </c>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="17" customFormat="1" ht="23.85">
+    <row r="49" spans="1:11" s="17" customFormat="1" ht="28">
       <c r="A49" s="3" t="s">
         <v>117</v>
       </c>
@@ -4847,7 +4926,7 @@
       </c>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" ht="23.85">
+    <row r="50" spans="1:11" ht="28">
       <c r="A50" s="3" t="s">
         <v>120</v>
       </c>
@@ -4872,7 +4951,7 @@
       </c>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" ht="23.85">
+    <row r="51" spans="1:11" ht="28">
       <c r="A51" s="3" t="s">
         <v>123</v>
       </c>
@@ -4897,7 +4976,7 @@
       </c>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" ht="23.85">
+    <row r="52" spans="1:11" ht="28">
       <c r="A52" s="3" t="s">
         <v>126</v>
       </c>
@@ -4922,7 +5001,7 @@
       </c>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" ht="23.85">
+    <row r="53" spans="1:11" ht="14">
       <c r="A53" s="3" t="s">
         <v>129</v>
       </c>
@@ -4947,7 +5026,7 @@
       </c>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" ht="23.85">
+    <row r="54" spans="1:11" ht="28">
       <c r="A54" s="3" t="s">
         <v>132</v>
       </c>
@@ -4974,7 +5053,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="23.85">
+    <row r="55" spans="1:11" ht="28">
       <c r="A55" s="3" t="s">
         <v>136</v>
       </c>
@@ -4999,7 +5078,7 @@
       </c>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" ht="23.85">
+    <row r="56" spans="1:11" ht="28">
       <c r="A56" s="3" t="s">
         <v>139</v>
       </c>
@@ -5024,7 +5103,7 @@
       </c>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" ht="14">
       <c r="A57" s="3" t="s">
         <v>142</v>
       </c>
@@ -5049,7 +5128,7 @@
       </c>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" ht="14">
       <c r="A58" s="3" t="s">
         <v>145</v>
       </c>
@@ -5074,7 +5153,7 @@
       </c>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" ht="14">
       <c r="A59" s="3" t="s">
         <v>147</v>
       </c>
@@ -5099,7 +5178,7 @@
       </c>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" ht="23.85">
+    <row r="60" spans="1:11" ht="28">
       <c r="A60" s="3" t="s">
         <v>149</v>
       </c>
@@ -5124,7 +5203,7 @@
       </c>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" ht="23.85">
+    <row r="61" spans="1:11" ht="28">
       <c r="A61" s="3" t="s">
         <v>152</v>
       </c>
@@ -5149,7 +5228,7 @@
       </c>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" ht="23.85">
+    <row r="62" spans="1:11" ht="28">
       <c r="A62" s="3" t="s">
         <v>155</v>
       </c>
@@ -5174,7 +5253,7 @@
       </c>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" ht="14">
       <c r="A63" s="3" t="s">
         <v>158</v>
       </c>
@@ -5640,19 +5719,19 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Select any team name you prefer." sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Select any team name you prefer." sqref="B2" xr:uid="{93AA5D26-42A2-4748-8C83-4FF166379586}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Please enter your name as it appears in Blackboard." sqref="B5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Please enter your name as it appears in Blackboard." sqref="B5" xr:uid="{358A4AFF-AFF4-9D42-B332-7C783E42E1EE}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initials" prompt="Please enter 2 or 3 capital letters that will represent you  in the &quot;Assigned To&quot; column on each Sprint Backlog tab of this spreadsheet." sqref="H5" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initials" prompt="Please enter 2 or 3 capital letters that will represent you  in the &quot;Assigned To&quot; column on each Sprint Backlog tab of this spreadsheet." sqref="H5" xr:uid="{D721C3EB-FF21-9F48-9BC8-B05B3DF98254}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Student ID" prompt="Please enter your UTA student ID number." sqref="I5" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Student ID" prompt="Please enter your UTA student ID number." sqref="I5" xr:uid="{92344B9B-3659-A84E-A99A-AC01C88F8743}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5692,19 +5771,19 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B17" sqref="B17:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -5794,7 +5873,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -5808,8 +5887,8 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
-        <v>1</v>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
+        <v>6</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5826,8 +5905,8 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5844,8 +5923,8 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5862,8 +5941,8 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5880,8 +5959,8 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5898,12 +5977,12 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -5916,8 +5995,8 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5963,51 +6042,103 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
       <c r="D17" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="28"/>
+        <v>186</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="28"/>
+      <c r="B20" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
         <v>5</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="28"/>
+      <c r="B21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="28"/>
+      <c r="B22" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
@@ -6647,7 +6778,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D20:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6669,7 +6800,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C17:C100</xm:sqref>
+          <xm:sqref>C23:C100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
@@ -6678,7 +6809,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B23:B100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6690,20 +6821,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -6796,7 +6927,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -6810,8 +6941,8 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
-        <v>1</v>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
+        <v>2</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6828,8 +6959,8 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6846,8 +6977,8 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6864,8 +6995,8 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6882,8 +7013,8 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6900,12 +7031,12 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -6918,8 +7049,8 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6965,19 +7096,35 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
       <c r="D17" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="28"/>
+        <v>193</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
@@ -7680,7 +7827,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B19:B100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7696,16 +7843,16 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -7812,7 +7959,7 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
         <v>1</v>
       </c>
       <c r="C8" s="18">
@@ -7830,7 +7977,7 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="18">
@@ -7848,7 +7995,7 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C10" s="18">
@@ -7866,7 +8013,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="18">
@@ -7884,7 +8031,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="18">
@@ -7902,7 +8049,7 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" s="18">
@@ -7920,7 +8067,7 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14" s="18">
@@ -8698,16 +8845,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -8813,7 +8960,7 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
         <v>1</v>
       </c>
       <c r="C8" s="18">
@@ -8831,7 +8978,7 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="18">
@@ -8849,7 +8996,7 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C10" s="18">
@@ -8867,7 +9014,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="18">
@@ -8885,7 +9032,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="18">
@@ -8903,7 +9050,7 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" s="18">
@@ -8921,7 +9068,7 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14" s="18">
@@ -9699,16 +9846,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -9815,7 +9962,7 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
         <v>1</v>
       </c>
       <c r="C8" s="18">
@@ -9833,7 +9980,7 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="18">
@@ -9851,7 +9998,7 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C10" s="18">
@@ -9869,7 +10016,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="18">
@@ -9887,7 +10034,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="18">
@@ -9905,7 +10052,7 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" s="18">
@@ -9923,7 +10070,7 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14" s="18">
@@ -10701,16 +10848,16 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="20" customFormat="1" ht="17.45">
+    <row r="1" spans="1:1024" s="20" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
@@ -10817,7 +10964,7 @@
         <v>168</v>
       </c>
       <c r="B8" s="18">
-        <f>B7-C8</f>
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
         <v>1</v>
       </c>
       <c r="C8" s="18">
@@ -10835,7 +10982,7 @@
         <v>169</v>
       </c>
       <c r="B9" s="18">
-        <f>B8-C9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="18">
@@ -10853,7 +11000,7 @@
         <v>170</v>
       </c>
       <c r="B10" s="18">
-        <f>B9-C10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C10" s="18">
@@ -10871,7 +11018,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="18">
-        <f>B10-C11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="18">
@@ -10889,7 +11036,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="18">
-        <f>B11-C12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="18">
@@ -10907,7 +11054,7 @@
         <v>173</v>
       </c>
       <c r="B13" s="18">
-        <f>B12-C13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" s="18">
@@ -10925,7 +11072,7 @@
         <v>174</v>
       </c>
       <c r="B14" s="18">
-        <f>B13-C14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14" s="18">

</xml_diff>